<commit_message>
added srt buttons to gui. Now i need to add function to buttons
</commit_message>
<xml_diff>
--- a/SelectiveReminding/ScoreSheet.xlsx
+++ b/SelectiveReminding/ScoreSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonsteffener/Documents/GitHub/CognitiveTasks/SelectiveReminding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{73D873A9-6936-F54D-A27A-2776C788B6EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC7715A-F89D-7D4A-8A05-EADBCCE3FE12}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15720" xr2:uid="{E9D2D987-B359-D747-84E6-77629BE60A3E}"/>
+    <workbookView xWindow="6060" yWindow="940" windowWidth="27640" windowHeight="15720" xr2:uid="{E9D2D987-B359-D747-84E6-77629BE60A3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,9 +66,6 @@
     <t>RACCOON</t>
   </si>
   <si>
-    <t>Recall1</t>
-  </si>
-  <si>
     <t>Recall2</t>
   </si>
   <si>
@@ -103,6 +100,9 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>Recall 1</t>
   </si>
 </sst>
 </file>
@@ -164,14 +164,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -490,55 +490,55 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="45" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.83203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="5.83203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
     <col min="3" max="10" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>22</v>
+      <c r="J2" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -554,7 +554,7 @@
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -570,7 +570,7 @@
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -586,7 +586,7 @@
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -602,7 +602,7 @@
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -618,7 +618,7 @@
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -634,7 +634,7 @@
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="4">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -650,7 +650,7 @@
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="A10" s="4">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -666,7 +666,7 @@
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="4">
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -682,8 +682,8 @@
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>23</v>
+      <c r="A12" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>10</v>
@@ -698,8 +698,8 @@
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>24</v>
+      <c r="A13" s="4" t="s">
+        <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>11</v>
@@ -714,8 +714,8 @@
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>25</v>
+      <c r="A14" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
made srt 6 trials
</commit_message>
<xml_diff>
--- a/SelectiveReminding/ScoreSheet.xlsx
+++ b/SelectiveReminding/ScoreSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonsteffener/Documents/GitHub/CognitiveTasks/SelectiveReminding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D6DA4A-A39F-9A41-ABDE-ED20CDFDC725}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AC7C8D-F900-2743-AC6F-0E8A504407FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="15720" xr2:uid="{E9D2D987-B359-D747-84E6-77629BE60A3E}"/>
   </bookViews>
@@ -78,12 +78,6 @@
     <t>Recall5</t>
   </si>
   <si>
-    <t>5 Min Delay</t>
-  </si>
-  <si>
-    <t>30 Min Delay</t>
-  </si>
-  <si>
     <t>Participant ID</t>
   </si>
   <si>
@@ -109,6 +103,12 @@
   </si>
   <si>
     <t>After the participant recalls the list, type in the Index of all words recalled and press return.</t>
+  </si>
+  <si>
+    <t>Recall 6</t>
+  </si>
+  <si>
+    <t>15 Min Delay</t>
   </si>
 </sst>
 </file>
@@ -556,7 +556,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="45" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -568,15 +568,16 @@
   <sheetData>
     <row r="1" spans="1:10" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>20</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
@@ -589,13 +590,13 @@
     </row>
     <row r="3" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>13</v>
@@ -610,13 +611,13 @@
         <v>16</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -765,7 +766,7 @@
     </row>
     <row r="13" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>10</v>
@@ -781,7 +782,7 @@
     </row>
     <row r="14" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>11</v>
@@ -797,7 +798,7 @@
     </row>
     <row r="15" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
updated SRT word lists
</commit_message>
<xml_diff>
--- a/SelectiveReminding/ScoreSheet.xlsx
+++ b/SelectiveReminding/ScoreSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonsteffener/Documents/GitHub/CognitiveTasks/SelectiveReminding/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AC7C8D-F900-2743-AC6F-0E8A504407FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7460CB23-2EC0-994E-9416-9FAB25ABD85F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="460" windowWidth="27640" windowHeight="15720" xr2:uid="{E9D2D987-B359-D747-84E6-77629BE60A3E}"/>
+    <workbookView xWindow="5440" yWindow="460" windowWidth="27640" windowHeight="15720" xr2:uid="{E9D2D987-B359-D747-84E6-77629BE60A3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,42 +30,6 @@
     <t>Word</t>
   </si>
   <si>
-    <t>DOG</t>
-  </si>
-  <si>
-    <t>FOX</t>
-  </si>
-  <si>
-    <t>HORSE</t>
-  </si>
-  <si>
-    <t>BUFFALO</t>
-  </si>
-  <si>
-    <t>LION</t>
-  </si>
-  <si>
-    <t>RHINOCEROS</t>
-  </si>
-  <si>
-    <t>ELEPHANT</t>
-  </si>
-  <si>
-    <t>ANTELOPE</t>
-  </si>
-  <si>
-    <t>BEAR</t>
-  </si>
-  <si>
-    <t>LAMB</t>
-  </si>
-  <si>
-    <t>RAT</t>
-  </si>
-  <si>
-    <t>RACCOON</t>
-  </si>
-  <si>
     <t>Recall2</t>
   </si>
   <si>
@@ -84,9 +48,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Recog</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -109,6 +70,45 @@
   </si>
   <si>
     <t>15 Min Delay</t>
+  </si>
+  <si>
+    <t>THROW</t>
+  </si>
+  <si>
+    <t>LILY</t>
+  </si>
+  <si>
+    <t>FILM</t>
+  </si>
+  <si>
+    <t>DISCREET</t>
+  </si>
+  <si>
+    <t>LOFT</t>
+  </si>
+  <si>
+    <t>BEEF</t>
+  </si>
+  <si>
+    <t>STREET</t>
+  </si>
+  <si>
+    <t>HELMET</t>
+  </si>
+  <si>
+    <t>SNAKE</t>
+  </si>
+  <si>
+    <t>DUG</t>
+  </si>
+  <si>
+    <t>PACK</t>
+  </si>
+  <si>
+    <t>TIN</t>
+  </si>
+  <si>
+    <t>INTRUSIONS</t>
   </si>
 </sst>
 </file>
@@ -139,7 +139,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -191,19 +191,6 @@
     <border>
       <left/>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -236,9 +223,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,31 +538,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157D929B-B352-C74D-95F1-5BBD6C092F5B}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.83203125" defaultRowHeight="45" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.33203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="10" width="8.6640625" customWidth="1"/>
+    <col min="3" max="9" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:10" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="8"/>
@@ -586,46 +571,42 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
-      <c r="J2" s="9"/>
-    </row>
-    <row r="3" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="I3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>1</v>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -634,14 +615,13 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>2</v>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -650,14 +630,13 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>3</v>
+      <c r="B6" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
@@ -666,14 +645,13 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>4</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>4</v>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -682,14 +660,13 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>5</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
+      <c r="B8" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -698,14 +675,13 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>6</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>6</v>
+      <c r="B9" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -714,14 +690,13 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>7</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>7</v>
+      <c r="B10" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -730,14 +705,13 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>8</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>8</v>
+      <c r="B11" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -746,14 +720,13 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>9</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>9</v>
+      <c r="B12" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -762,14 +735,13 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -778,14 +750,13 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -794,14 +765,13 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:9" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -810,11 +780,15 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
+    </row>
+    <row r="17" spans="2:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B2:I2"/>
   </mergeCells>
   <pageMargins left="0.45" right="0.45" top="0.75" bottom="0.75" header="0" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>